<commit_message>
fix một số lỗi do merge gây ra
</commit_message>
<xml_diff>
--- a/Auto_Import_Device/Version_3/sample_input_v3.xlsx
+++ b/Auto_Import_Device/Version_3/sample_input_v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\netbox-import-tool\Auto_Import_Device\Version_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC467CF-19A7-4752-BBD3-DBC4E7E91EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B51BAD-753C-4E26-B299-14BDC42452DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="66">
   <si>
     <t>Mô tả cấu hỉnh</t>
   </si>
@@ -144,12 +144,6 @@
     <t>005/22/TE-005/STS</t>
   </si>
   <si>
-    <t>006/22/TE-006/STS</t>
-  </si>
-  <si>
-    <t>007/22/TE-007/STS</t>
-  </si>
-  <si>
     <t>01TE001ST</t>
   </si>
   <si>
@@ -192,12 +186,6 @@
     <t>14TE014ST</t>
   </si>
   <si>
-    <t>15TE015ST</t>
-  </si>
-  <si>
-    <t>16TE016ST</t>
-  </si>
-  <si>
     <t>test import</t>
   </si>
   <si>
@@ -219,26 +207,33 @@
     <t>SVXR03</t>
   </si>
   <si>
-    <t>SVXR02</t>
-  </si>
-  <si>
-    <t>SVXR01</t>
-  </si>
-  <si>
     <t>SV Test 1</t>
   </si>
   <si>
     <t>SV Test 2</t>
+  </si>
+  <si>
+    <t>DGX A100</t>
+  </si>
+  <si>
+    <t>001/21/MB-001/3H-NTC</t>
+  </si>
+  <si>
+    <t>8/1/2021</t>
+  </si>
+  <si>
+    <t>15te70023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0\ &quot;W&quot;"/>
+    <numFmt numFmtId="165" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,8 +292,14 @@
       <name val="TimesNewRomanPSMT"/>
       <charset val="163"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,8 +324,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -347,12 +354,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -435,32 +479,90 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -745,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -758,7 +860,7 @@
     <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.21875" style="29" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="52" bestFit="1" customWidth="1"/>
@@ -826,17 +928,17 @@
         <v>23</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="25" t="s">
         <v>5</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="L2" s="23" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -880,17 +982,17 @@
         <v>23</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="25" t="s">
         <v>5</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="L4" s="23" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -934,17 +1036,17 @@
         <v>23</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="25" t="s">
         <v>4</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="L6" s="23" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -988,7 +1090,7 @@
         <v>23</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I8" s="12"/>
       <c r="J8" s="25" t="s">
@@ -996,7 +1098,7 @@
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="23" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1040,17 +1142,17 @@
         <v>23</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I10" s="12"/>
       <c r="J10" s="25" t="s">
         <v>4</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="L10" s="23" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1094,7 +1196,7 @@
         <v>23</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="25" t="s">
@@ -1102,7 +1204,7 @@
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="23" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1144,17 +1246,17 @@
         <v>23</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I14" s="14"/>
       <c r="J14" s="25" t="s">
         <v>4</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="L14" s="23" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1273,7 +1375,7 @@
         <v>23</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D21" s="19" t="s">
         <v>3</v>
@@ -1288,7 +1390,7 @@
         <v>24</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I21" s="19"/>
       <c r="J21" s="28" t="s">
@@ -1296,7 +1398,7 @@
       </c>
       <c r="K21" s="2"/>
       <c r="L21" s="23" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1307,7 +1409,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D22" s="19" t="s">
         <v>3</v>
@@ -1322,17 +1424,17 @@
         <v>24</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I22" s="19"/>
       <c r="J22" s="28" t="s">
         <v>19</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="L22" s="23" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1342,33 +1444,33 @@
       <c r="B23" s="3">
         <v>21</v>
       </c>
-      <c r="C23" s="34" t="s">
+      <c r="C23" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="D23" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="F23" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="H23" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="I23" s="34"/>
-      <c r="J23" s="33" t="s">
+      <c r="H23" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="I23" s="30"/>
+      <c r="J23" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="K23" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="L23" s="30" t="s">
-        <v>58</v>
+      <c r="K23" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="L23" s="38" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1378,16 +1480,16 @@
       <c r="B24" s="3">
         <v>20</v>
       </c>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="38"/>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="6" t="s">
@@ -1397,7 +1499,7 @@
         <v>19</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>3</v>
@@ -1412,7 +1514,7 @@
         <v>24</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I25" s="3"/>
       <c r="J25" s="25" t="s">
@@ -1420,7 +1522,7 @@
       </c>
       <c r="K25" s="2"/>
       <c r="L25" s="23" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1449,7 +1551,7 @@
         <v>17</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>3</v>
@@ -1464,7 +1566,7 @@
         <v>24</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="25" t="s">
@@ -1472,7 +1574,7 @@
       </c>
       <c r="K27" s="2"/>
       <c r="L27" s="23" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1482,33 +1584,33 @@
       <c r="B28" s="3">
         <v>16</v>
       </c>
-      <c r="C28" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" s="34" t="s">
+      <c r="C28" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="34" t="s">
+      <c r="E28" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="F28" s="37" t="s">
+      <c r="F28" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="G28" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="H28" s="36" t="s">
+      <c r="G28" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="H28" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="I28" s="34"/>
+      <c r="J28" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="K28" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="I28" s="31"/>
-      <c r="J28" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="K28" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="L28" s="30" t="s">
-        <v>58</v>
+      <c r="L28" s="38" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1518,16 +1620,16 @@
       <c r="B29" s="3">
         <v>15</v>
       </c>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="33"/>
-      <c r="K29" s="32"/>
-      <c r="L29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="38"/>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="6" t="s">
@@ -1536,16 +1638,16 @@
       <c r="B30" s="3">
         <v>14</v>
       </c>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="32"/>
-      <c r="L30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="38"/>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="6" t="s">
@@ -1554,16 +1656,16 @@
       <c r="B31" s="3">
         <v>13</v>
       </c>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="32"/>
-      <c r="L31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="31"/>
+      <c r="L31" s="38"/>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="6" t="s">
@@ -1572,33 +1674,33 @@
       <c r="B32" s="3">
         <v>12</v>
       </c>
-      <c r="C32" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="D32" s="34" t="s">
+      <c r="C32" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="34" t="s">
+      <c r="E32" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="F32" s="37" t="s">
+      <c r="F32" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="G32" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="H32" s="36" t="s">
+      <c r="G32" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="H32" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="I32" s="34"/>
+      <c r="J32" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="K32" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="L32" s="38" t="s">
         <v>54</v>
-      </c>
-      <c r="I32" s="31"/>
-      <c r="J32" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="K32" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="L32" s="30" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -1608,16 +1710,16 @@
       <c r="B33" s="3">
         <v>11</v>
       </c>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="30"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="31"/>
+      <c r="L33" s="38"/>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="6" t="s">
@@ -1626,16 +1728,16 @@
       <c r="B34" s="3">
         <v>10</v>
       </c>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="33"/>
-      <c r="K34" s="32"/>
-      <c r="L34" s="30"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="40"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="41"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="43"/>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="6" t="s">
@@ -1644,16 +1746,32 @@
       <c r="B35" s="3">
         <v>9</v>
       </c>
-      <c r="C35" s="34"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="34"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="33"/>
-      <c r="K35" s="32"/>
-      <c r="L35" s="30"/>
+      <c r="C35" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="G35" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="H35" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="I35" s="49"/>
+      <c r="J35" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="K35" s="53"/>
+      <c r="L35" s="56" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="6" t="s">
@@ -1662,34 +1780,16 @@
       <c r="B36" s="3">
         <v>8</v>
       </c>
-      <c r="C36" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="D36" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="E36" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="F36" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="G36" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="H36" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="I36" s="31"/>
-      <c r="J36" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="K36" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="L36" s="30" t="s">
-        <v>58</v>
-      </c>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="45"/>
+      <c r="H36" s="47"/>
+      <c r="I36" s="50"/>
+      <c r="J36" s="48"/>
+      <c r="K36" s="54"/>
+      <c r="L36" s="57"/>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="6" t="s">
@@ -1698,16 +1798,16 @@
       <c r="B37" s="3">
         <v>7</v>
       </c>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="31"/>
-      <c r="J37" s="33"/>
-      <c r="K37" s="32"/>
-      <c r="L37" s="30"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="45"/>
+      <c r="H37" s="47"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="48"/>
+      <c r="K37" s="54"/>
+      <c r="L37" s="57"/>
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="6" t="s">
@@ -1716,16 +1816,16 @@
       <c r="B38" s="3">
         <v>6</v>
       </c>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="34"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="31"/>
-      <c r="J38" s="33"/>
-      <c r="K38" s="32"/>
-      <c r="L38" s="30"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="45"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="48"/>
+      <c r="K38" s="54"/>
+      <c r="L38" s="57"/>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="6" t="s">
@@ -1734,16 +1834,16 @@
       <c r="B39" s="3">
         <v>5</v>
       </c>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="37"/>
-      <c r="G39" s="34"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="31"/>
-      <c r="J39" s="33"/>
-      <c r="K39" s="32"/>
-      <c r="L39" s="30"/>
+      <c r="C39" s="45"/>
+      <c r="D39" s="45"/>
+      <c r="E39" s="45"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="45"/>
+      <c r="H39" s="47"/>
+      <c r="I39" s="50"/>
+      <c r="J39" s="48"/>
+      <c r="K39" s="54"/>
+      <c r="L39" s="57"/>
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="6" t="s">
@@ -1752,34 +1852,16 @@
       <c r="B40" s="3">
         <v>4</v>
       </c>
-      <c r="C40" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="D40" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="E40" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="F40" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="G40" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="H40" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="I40" s="31"/>
-      <c r="J40" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="K40" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="L40" s="30" t="s">
-        <v>58</v>
-      </c>
+      <c r="C40" s="45"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="45"/>
+      <c r="F40" s="38"/>
+      <c r="G40" s="45"/>
+      <c r="H40" s="47"/>
+      <c r="I40" s="51"/>
+      <c r="J40" s="48"/>
+      <c r="K40" s="55"/>
+      <c r="L40" s="58"/>
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="6" t="s">
@@ -1788,16 +1870,16 @@
       <c r="B41" s="3">
         <v>3</v>
       </c>
-      <c r="C41" s="34"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="37"/>
-      <c r="G41" s="34"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="31"/>
-      <c r="J41" s="33"/>
-      <c r="K41" s="32"/>
-      <c r="L41" s="30"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="40"/>
+      <c r="I41" s="44"/>
+      <c r="J41" s="41"/>
+      <c r="K41" s="42"/>
+      <c r="L41" s="43"/>
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="6" t="s">
@@ -1806,16 +1888,16 @@
       <c r="B42" s="3">
         <v>2</v>
       </c>
-      <c r="C42" s="34"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="37"/>
-      <c r="G42" s="34"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="31"/>
-      <c r="J42" s="33"/>
-      <c r="K42" s="32"/>
-      <c r="L42" s="30"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="40"/>
+      <c r="I42" s="44"/>
+      <c r="J42" s="41"/>
+      <c r="K42" s="42"/>
+      <c r="L42" s="43"/>
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="6" t="s">
@@ -1824,57 +1906,48 @@
       <c r="B43" s="3">
         <v>1</v>
       </c>
-      <c r="C43" s="34"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="34"/>
-      <c r="F43" s="37"/>
-      <c r="G43" s="34"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="31"/>
-      <c r="J43" s="33"/>
-      <c r="K43" s="32"/>
-      <c r="L43" s="30"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="41"/>
+      <c r="K43" s="42"/>
+      <c r="L43" s="43"/>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="90">
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="K38:K39"/>
-    <mergeCell ref="K28:K29"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="K32:K33"/>
-    <mergeCell ref="K34:K35"/>
-    <mergeCell ref="K36:K37"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="J36:J37"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="H36:H37"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="I36:I37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="J32:J33"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="J34:J35"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="H32:H33"/>
+  <mergeCells count="50">
+    <mergeCell ref="C35:C40"/>
+    <mergeCell ref="D35:D40"/>
+    <mergeCell ref="E35:E40"/>
+    <mergeCell ref="F35:F40"/>
+    <mergeCell ref="G35:G40"/>
+    <mergeCell ref="H35:H40"/>
+    <mergeCell ref="J35:J40"/>
+    <mergeCell ref="K35:K40"/>
+    <mergeCell ref="I35:I40"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="L28:L29"/>
+    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="L32:L33"/>
+    <mergeCell ref="L35:L40"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="J30:J31"/>
     <mergeCell ref="I32:I33"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="C28:C29"/>
@@ -1887,47 +1960,16 @@
     <mergeCell ref="H30:H31"/>
     <mergeCell ref="I30:I31"/>
     <mergeCell ref="E30:E31"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="J42:J43"/>
-    <mergeCell ref="K42:K43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="H40:H41"/>
-    <mergeCell ref="I40:I41"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="G42:G43"/>
-    <mergeCell ref="H42:H43"/>
-    <mergeCell ref="I42:I43"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="J40:J41"/>
-    <mergeCell ref="K40:K41"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="L36:L37"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="L40:L41"/>
-    <mergeCell ref="L42:L43"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="L28:L29"/>
-    <mergeCell ref="L30:L31"/>
-    <mergeCell ref="L32:L33"/>
-    <mergeCell ref="L34:L35"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="D32:D33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>